<commit_message>
Update Sszs excel template, consistent Bigdecimal value
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sszs_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sszs_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8765F5B-3ED4-4FF7-8925-1F170C7B96FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8247FF3-ED7D-4F65-85C3-072F93CD1F83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19320" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1070,37 +1070,25 @@
   <dimension ref="B1:AG62"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.85546875" style="1" customWidth="1"/>
+    <col min="6" max="11" width="4" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="4" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="4.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7.5703125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="2.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="3" style="1" customWidth="1"/>
-    <col min="25" max="25" width="3.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="3.140625" style="1" customWidth="1"/>
+    <col min="17" max="21" width="5.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="3.85546875" style="1" customWidth="1"/>
+    <col min="25" max="26" width="5.7109375" style="1" customWidth="1"/>
     <col min="27" max="27" width="3.28515625" style="1" customWidth="1"/>
     <col min="28" max="28" width="3.140625" style="1" customWidth="1"/>
     <col min="29" max="29" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1746,10 +1734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1795,7 +1779,20 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1987,16 +1984,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947F1741-2986-4B63-8B5C-D0468C671233}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -2004,15 +2000,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD45C59E-C13E-4B92-9551-AE1790848EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2029,12 +2025,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Sszs: fix column C,D,E,P,V (#1644)
* Sszs: fix column C,D,E,P,V

* Update Sszs excel template, consistent Bigdecimal value

* update JUnit test

---------

Co-authored-by: Marius Heine <m.heine@geprog.com>
</commit_message>
<xml_diff>
--- a/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sszs_vorlage.xlsx
+++ b/java/bundles/org.eclipse.set.feature/rootdir/data/export/excel/sszs_vorlage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ws-intern\PlanPro-Git\eclipse-set\java\bundles\org.eclipse.set.feature\rootdir\data\export\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8765F5B-3ED4-4FF7-8925-1F170C7B96FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8247FF3-ED7D-4F65-85C3-072F93CD1F83}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="19320" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1070,37 +1070,25 @@
   <dimension ref="B1:AG62"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+      <selection activeCell="Y9" sqref="Y9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="5.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="3.42578125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="4.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="5.85546875" style="1" customWidth="1"/>
+    <col min="6" max="11" width="4" style="1" customWidth="1"/>
     <col min="12" max="12" width="7.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" style="1" customWidth="1"/>
+    <col min="13" max="14" width="4" style="1" customWidth="1"/>
     <col min="15" max="15" width="6.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="3.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="4.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5" style="1" customWidth="1"/>
-    <col min="21" max="21" width="4.85546875" style="1" customWidth="1"/>
-    <col min="22" max="22" width="7.5703125" style="1" customWidth="1"/>
-    <col min="23" max="23" width="2.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="3" style="1" customWidth="1"/>
-    <col min="25" max="25" width="3.28515625" style="1" customWidth="1"/>
-    <col min="26" max="26" width="3.140625" style="1" customWidth="1"/>
+    <col min="17" max="21" width="5.7109375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="6.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="5.7109375" style="1" customWidth="1"/>
+    <col min="24" max="24" width="3.85546875" style="1" customWidth="1"/>
+    <col min="25" max="26" width="5.7109375" style="1" customWidth="1"/>
     <col min="27" max="27" width="3.28515625" style="1" customWidth="1"/>
     <col min="28" max="28" width="3.140625" style="1" customWidth="1"/>
     <col min="29" max="29" width="8.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1746,10 +1734,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -1795,7 +1779,20 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100E758A0F93049BE4CAD441F10C0D8186D" ma:contentTypeVersion="5" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="fb340e34ecc5d059b634082484788e96">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="576ce185-3b2e-4f75-8b7c-efeb82226bea" xmlns:ns3="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae5cd419a40dc0c21009e0c04d2bd83e" ns2:_="" ns3:_="">
     <xsd:import namespace="576ce185-3b2e-4f75-8b7c-efeb82226bea"/>
@@ -1987,16 +1984,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{947F1741-2986-4B63-8B5C-D0468C671233}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
@@ -2004,15 +2000,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5FA61470-DD61-4999-8627-225AC049B66F}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD45C59E-C13E-4B92-9551-AE1790848EFA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2029,12 +2025,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1C5838C-81AB-4B9A-B282-4E4B57DAFB8B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>